<commit_message>
getting the graph prep ready
</commit_message>
<xml_diff>
--- a/notebooks/Data/2Nodes/OD.xlsx
+++ b/notebooks/Data/2Nodes/OD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasfuentes/ASL/ICU/notebooks/Data/2Nodes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BB21F2-DC25-E549-90EE-69F867CDE117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0722211-D34C-F043-BB52-E4BA64DED906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15800" xr2:uid="{5A1EB264-C47A-9A4B-BE1F-67BE568007CD}"/>
+    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="15800" xr2:uid="{5A1EB264-C47A-9A4B-BE1F-67BE568007CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>length</t>
   </si>
@@ -44,9 +44,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>is negative</t>
-  </si>
-  <si>
     <t>origin</t>
   </si>
   <si>
@@ -54,6 +51,12 @@
   </si>
   <si>
     <t>demand</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>isnegative</t>
   </si>
 </sst>
 </file>
@@ -405,23 +408,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2C9C56-0039-F448-9270-8D308784FB69}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -433,10 +436,13 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -450,7 +456,7 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -458,8 +464,11 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -473,13 +482,16 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3">
         <v>1</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solving the discrepancy between the two algos, starting to implement and test on larger graphs
</commit_message>
<xml_diff>
--- a/notebooks/Data/2Nodes/OD.xlsx
+++ b/notebooks/Data/2Nodes/OD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasfuentes/ASL/ICU/notebooks/Data/2Nodes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0722211-D34C-F043-BB52-E4BA64DED906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8187CE-24D9-FE42-A017-95BEF207BED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="15800" xr2:uid="{5A1EB264-C47A-9A4B-BE1F-67BE568007CD}"/>
+    <workbookView xWindow="13600" yWindow="940" windowWidth="13540" windowHeight="15800" xr2:uid="{5A1EB264-C47A-9A4B-BE1F-67BE568007CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +465,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>40</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>